<commit_message>
Finished the create_eos function
</commit_message>
<xml_diff>
--- a/Interpolación/data.xlsx
+++ b/Interpolación/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,73 +455,153 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8.606629658239049</v>
+        <v>5.923488777591456</v>
       </c>
       <c r="B3" t="n">
-        <v>11111.111111112</v>
+        <v>5263.157894737789</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>12.17161238900391</v>
+        <v>8.377078165834266</v>
       </c>
       <c r="B4" t="n">
-        <v>22222.222222223</v>
+        <v>10526.31578947458</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>14.90711984999875</v>
+        <v>10.25978352085181</v>
       </c>
       <c r="B5" t="n">
-        <v>33333.333333334</v>
+        <v>15789.47368421137</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>17.21325931647752</v>
+        <v>11.84697755518207</v>
       </c>
       <c r="B6" t="n">
-        <v>44444.444444445</v>
+        <v>21052.63157894816</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19.2450089729876</v>
+        <v>13.24532357065062</v>
       </c>
       <c r="B7" t="n">
-        <v>55555.555555556</v>
+        <v>26315.78947368494</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>21.08185106778925</v>
+        <v>14.50952500220039</v>
       </c>
       <c r="B8" t="n">
-        <v>66666.66666666701</v>
+        <v>31578.94736842173</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>22.77100170213247</v>
+        <v>15.67207819938771</v>
       </c>
       <c r="B9" t="n">
-        <v>77777.777777778</v>
+        <v>36842.10526315852</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>24.3432247780074</v>
+        <v>16.75415633166794</v>
       </c>
       <c r="B10" t="n">
-        <v>88888.88888888901</v>
+        <v>42105.26315789531</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>17.77046633277287</v>
+      </c>
+      <c r="B11" t="n">
+        <v>47368.4210526321</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>18.73171623163396</v>
+      </c>
+      <c r="B12" t="n">
+        <v>52631.57894736889</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>19.64598972515013</v>
+      </c>
+      <c r="B13" t="n">
+        <v>57894.73684210567</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>20.51956704170314</v>
+      </c>
+      <c r="B14" t="n">
+        <v>63157.89473684246</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>21.35744251723963</v>
+      </c>
+      <c r="B15" t="n">
+        <v>68421.05263157927</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>22.16366554014566</v>
+      </c>
+      <c r="B16" t="n">
+        <v>73684.21052631605</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>22.94157338705621</v>
+      </c>
+      <c r="B17" t="n">
+        <v>78947.36842105283</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>23.69395511036372</v>
+      </c>
+      <c r="B18" t="n">
+        <v>84210.52631578963</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>24.42316990216823</v>
+      </c>
+      <c r="B19" t="n">
+        <v>89473.68421052642</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>25.13123449750174</v>
+      </c>
+      <c r="B20" t="n">
+        <v>94736.8421052632</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>25.81988897471611</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B21" t="n">
         <v>100000</v>
       </c>
     </row>

</xml_diff>